<commit_message>
fixed after splitting to Export/Exporter and Import/Importer
</commit_message>
<xml_diff>
--- a/test/exportSample/toBeImported.xlsx
+++ b/test/exportSample/toBeImported.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>en</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>doigt</t>
+  </si>
+  <si>
+    <t>base</t>
   </si>
 </sst>
 </file>
@@ -383,51 +386,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Now indexing both JSON and xlsx files when importing to make sure that the same key is not used twice with the same base.
Testing a bit more.
</commit_message>
<xml_diff>
--- a/test/exportSample/toBeImported.xlsx
+++ b/test/exportSample/toBeImported.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>en</t>
   </si>
@@ -22,31 +22,37 @@
     <t>fr</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>alphabet</t>
-  </si>
-  <si>
-    <t>bateau</t>
-  </si>
-  <si>
-    <t>chapeau</t>
-  </si>
-  <si>
-    <t>doigt</t>
-  </si>
-  <si>
     <t>base</t>
+  </si>
+  <si>
+    <t>es</t>
+  </si>
+  <si>
+    <t>jeter</t>
+  </si>
+  <si>
+    <t>botar</t>
+  </si>
+  <si>
+    <t>chien</t>
+  </si>
+  <si>
+    <t>perro</t>
+  </si>
+  <si>
+    <t>dog</t>
+  </si>
+  <si>
+    <t>avion</t>
+  </si>
+  <si>
+    <t>avión</t>
+  </si>
+  <si>
+    <t>plane</t>
+  </si>
+  <si>
+    <t>throw</t>
   </si>
 </sst>
 </file>
@@ -386,70 +392,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>